<commit_message>
Grants high scenarios projects
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Grants_Input.xlsx
+++ b/src/main/java/resources/Grants_Input.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="5865" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14150" windowHeight="5870"/>
   </bookViews>
   <sheets>
     <sheet name="Select Grant type" sheetId="9" r:id="rId1"/>
     <sheet name="DG login details" sheetId="10" r:id="rId2"/>
     <sheet name="Select DG Grant Type" sheetId="11" r:id="rId3"/>
+    <sheet name="Step 1" sheetId="12" r:id="rId4"/>
+    <sheet name="My Grants" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Grant Type</t>
   </si>
@@ -44,20 +46,89 @@
     <t>Testing1</t>
   </si>
   <si>
-    <t>pangiaernesto@hotmail.com</t>
-  </si>
-  <si>
-    <t>District Grants [2019/2020]</t>
-  </si>
-  <si>
     <t>District Grant Type</t>
+  </si>
+  <si>
+    <t>Project_Name</t>
+  </si>
+  <si>
+    <t>Test_Grant_Project</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Primary_Contact_Role</t>
+  </si>
+  <si>
+    <t>PrimaryContact_sponsor</t>
+  </si>
+  <si>
+    <t>Secondary_Contact_Sponsor</t>
+  </si>
+  <si>
+    <t>Secondary_Contact_District</t>
+  </si>
+  <si>
+    <t>Secondary_Contact_Club</t>
+  </si>
+  <si>
+    <t>Secondary_Contact_ID</t>
+  </si>
+  <si>
+    <t>Primary_Contact_Name</t>
+  </si>
+  <si>
+    <t>Secondary_Contact_Name</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Alloa</t>
+  </si>
+  <si>
+    <t>Michael Ericksen</t>
+  </si>
+  <si>
+    <t>MAD Cq</t>
+  </si>
+  <si>
+    <t>Step1</t>
+  </si>
+  <si>
+    <t>Step 1: Basic Information</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>10097662</t>
+  </si>
+  <si>
+    <t>My Grants Page Title</t>
+  </si>
+  <si>
+    <t>My Grants</t>
+  </si>
+  <si>
+    <t>Grants_Session</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>p.ramage@pobroadband.co.uk</t>
+  </si>
+  <si>
+    <t>District Grants [2020/2021]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +144,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,10 +180,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -406,13 +495,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -420,10 +509,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -431,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -445,13 +534,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -459,9 +551,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -472,6 +564,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -483,9 +576,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -493,15 +586,127 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>